<commit_message>
- recentcollaboratorsbuilder.py (1) functionalized: turned simon's code into a separate function that returns a list of people and institutions. turned the csv/excel making codes into a separate function. - coa_template.xlsx: modified the template: unmerged the cells.
</commit_message>
<xml_diff>
--- a/regolith/templates/coa_template.xlsx
+++ b/regolith/templates/coa_template.xlsx
@@ -533,7 +533,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -551,7 +551,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -559,7 +559,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -567,7 +567,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -598,19 +602,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -651,7 +655,11 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -666,8 +674,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -768,15 +784,15 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.55"/>
@@ -909,7 +925,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="9" customFormat="true" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -919,71 +935,71 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="14" t="n">
+      <c r="D18" s="15" t="n">
         <v>42736</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="14" t="n">
+      <c r="D19" s="15" t="n">
         <v>42716</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" s="15" customFormat="true" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" s="16" customFormat="true" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" s="9" customFormat="true" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
@@ -992,90 +1008,90 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
+    <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="18" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="19"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="25"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="12"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
@@ -1087,283 +1103,283 @@
       <c r="E33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="19"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="33" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="32"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="34"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="31"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="33"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="31"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="33"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="26"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="26"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="27"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="26"/>
-    </row>
-    <row r="45" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="24"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="27"/>
+    </row>
+    <row r="45" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="12"/>
-    </row>
-    <row r="46" s="16" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="33" t="s">
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" s="17" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-    </row>
-    <row r="47" s="16" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="28" t="s">
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+    </row>
+    <row r="47" s="17" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="16" t="s">
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+    </row>
+    <row r="48" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="19"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="18" t="s">
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="19"/>
+      <c r="E49" s="37"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="22" t="s">
+      <c r="E50" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="23"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="25"/>
-    </row>
-    <row r="52" s="16" customFormat="true" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="24"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" s="35" customFormat="true" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" s="16" customFormat="true" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="33" t="s">
+    <row r="53" s="17" customFormat="true" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-    </row>
-    <row r="54" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="16" t="s">
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+    </row>
+    <row r="54" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E54" s="19"/>
-    </row>
-    <row r="55" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="16" t="s">
+      <c r="E54" s="20"/>
+    </row>
+    <row r="55" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E55" s="19"/>
+      <c r="E55" s="20"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="18" t="s">
+      <c r="A56" s="35"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E56" s="19"/>
+      <c r="E56" s="37"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="E57" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="D58" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E58" s="25" t="n">
+      <c r="E58" s="26" t="n">
         <v>42736</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="26"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="23"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="25"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="25"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="34"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="37"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="41"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="14">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
@@ -1378,14 +1394,6 @@
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="A53:E53"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A51" type="list">

</xml_diff>